<commit_message>
990114 - major updates on management file
</commit_message>
<xml_diff>
--- a/Main/shares template.xlsx
+++ b/Main/shares template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="715"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="715" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="دارایی فعلی" sheetId="3" r:id="rId1"/>
@@ -12,6 +12,9 @@
     <sheet name="تاریخچه خرید" sheetId="6" r:id="rId3"/>
     <sheet name="تاریخچه فروش" sheetId="4" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
@@ -272,7 +275,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -321,6 +324,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="45">
     <border>
@@ -921,7 +930,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1012,19 +1021,64 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="9" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="9" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="9" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="9" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1036,76 +1090,49 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1168,6 +1195,9 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1177,9 +1207,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1210,9 +1237,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="27" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1244,6 +1268,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1294,6 +1321,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1304,24 +1349,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1330,6 +1357,15 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1339,6 +1375,12 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1384,25 +1426,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="9" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1421,6 +1451,35 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="مدیریت سرمایه"/>
+      <sheetName val="محاسبه مدیریت سرمایه"/>
+      <sheetName val="پرتفوی"/>
+      <sheetName val="تحلیل"/>
+      <sheetName val="تاریخچه خرید"/>
+      <sheetName val="تاریخچه فروش"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="5">
+          <cell r="B5">
+            <v>1510830609</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1712,9 +1771,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N21" sqref="N21"/>
+      <selection pane="bottomLeft" activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1734,38 +1793,38 @@
   <sheetData>
     <row r="1" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:19" ht="19.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="156" t="s">
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="158"/>
-      <c r="M2" s="157"/>
-      <c r="N2" s="42" t="s">
+      <c r="L2" s="48"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="43" t="s">
+      <c r="O2" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="33" t="s">
+      <c r="P2" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="43" t="s">
+      <c r="Q2" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="R2" s="44" t="s">
+      <c r="R2" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="32" t="s">
+      <c r="S2" s="42" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1797,112 +1856,120 @@
       <c r="J3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="160" t="s">
+      <c r="K3" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="L3" s="161" t="s">
+      <c r="L3" s="33" t="s">
         <v>30</v>
       </c>
       <c r="M3" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="42"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="44"/>
-      <c r="S3" s="32"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="42"/>
     </row>
     <row r="4" spans="2:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="47">
+      <c r="B4" s="44">
         <f>IF(L4&gt;0, C4/L4,"RF")</f>
         <v>-9.9261059795819158</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="36">
         <f>(D4/Q4)-1</f>
         <v>-1</v>
       </c>
-      <c r="D4" s="48">
+      <c r="D4" s="45">
         <v>0</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="44">
         <f>IF(L4&gt;0, F4/L4,"RF")</f>
         <v>4.0291686922702974</v>
       </c>
-      <c r="F4" s="35">
+      <c r="F4" s="36">
         <f>(G4/Q4)-1</f>
         <v>0.40591634832010981</v>
       </c>
-      <c r="G4" s="48">
+      <c r="G4" s="45">
         <v>28706</v>
       </c>
-      <c r="H4" s="47">
+      <c r="H4" s="44">
         <f>IF(L4&gt;0, I4/L4,"RF")</f>
         <v>1.3179387457462326</v>
       </c>
-      <c r="I4" s="35">
+      <c r="I4" s="36">
         <f>(J4/Q4)-1</f>
         <v>0.13277500244881968</v>
       </c>
-      <c r="J4" s="48">
+      <c r="J4" s="45">
         <v>23129</v>
       </c>
-      <c r="K4" s="159">
+      <c r="K4" s="50">
         <f>IF(L4&gt;0, N4-M4*R4, 0)</f>
         <v>5440765</v>
       </c>
-      <c r="L4" s="162">
+      <c r="L4" s="51">
         <f>IF(1-(M4/Q4)&gt;0, 1-(M4/Q4), 0)</f>
         <v>0.10074444117935155</v>
       </c>
-      <c r="M4" s="50">
+      <c r="M4" s="46">
         <v>18361</v>
       </c>
-      <c r="N4" s="34">
+      <c r="N4" s="35">
         <f>R4*Q4</f>
         <v>54005610</v>
       </c>
-      <c r="O4" s="35">
+      <c r="O4" s="36">
         <f>IF( (Q4-M4)*R4/P4&gt;0, (Q4-M4)*R4/P4, "Risk free")</f>
-        <v>8.4531134616028219E-3</v>
-      </c>
-      <c r="P4" s="36">
-        <v>643640361</v>
-      </c>
-      <c r="Q4" s="36">
+        <v>3.6011747230890261E-3</v>
+      </c>
+      <c r="P4" s="37">
+        <f>'[1]مدیریت سرمایه'!$B$5</f>
+        <v>1510830609</v>
+      </c>
+      <c r="Q4" s="37">
         <f>(SUM('تاریخچه خرید'!M4:M17)-SUMPRODUCT('تاریخچه فروش'!G4:G7*'تاریخچه فروش'!F4:F7))/R4</f>
         <v>20418</v>
       </c>
-      <c r="R4" s="45">
+      <c r="R4" s="39">
         <f>SUM('تاریخچه خرید'!Q4:Q17)-SUM('تاریخچه فروش'!G4:G11)</f>
         <v>2645</v>
       </c>
-      <c r="S4" s="46" t="s">
+      <c r="S4" s="34" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="47"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="159"/>
-      <c r="L5" s="162"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="36"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="46"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="39"/>
+      <c r="S5" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="K4:K5"/>
@@ -1911,24 +1978,17 @@
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="L4:L5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
     <mergeCell ref="B2:J2"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="R4:R5"/>
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="S4:S5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
@@ -1962,44 +2022,44 @@
   <sheetData>
     <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:21" ht="19.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="64" t="s">
+      <c r="C2" s="68"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="78" t="s">
+      <c r="G2" s="69"/>
+      <c r="H2" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="79"/>
-      <c r="J2" s="105" t="s">
+      <c r="I2" s="85"/>
+      <c r="J2" s="110" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="106"/>
-      <c r="L2" s="68" t="s">
+      <c r="K2" s="111"/>
+      <c r="L2" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="69"/>
-      <c r="N2" s="74" t="s">
+      <c r="M2" s="75"/>
+      <c r="N2" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="75"/>
-      <c r="P2" s="37" t="s">
+      <c r="O2" s="81"/>
+      <c r="P2" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="74" t="s">
+      <c r="Q2" s="53"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="T2" s="75"/>
-      <c r="U2" s="64" t="s">
+      <c r="T2" s="81"/>
+      <c r="U2" s="70" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2013,7 +2073,7 @@
       <c r="D3" s="4">
         <v>4</v>
       </c>
-      <c r="E3" s="71"/>
+      <c r="E3" s="77"/>
       <c r="F3" s="5" t="s">
         <v>13</v>
       </c>
@@ -2059,401 +2119,401 @@
       <c r="T3" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="U3" s="65"/>
+      <c r="U3" s="71"/>
     </row>
     <row r="4" spans="1:21" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27"/>
-      <c r="B4" s="53">
+      <c r="B4" s="57">
         <v>1</v>
       </c>
-      <c r="C4" s="55">
+      <c r="C4" s="59">
         <v>2</v>
       </c>
-      <c r="D4" s="57">
+      <c r="D4" s="61">
         <v>3</v>
       </c>
-      <c r="E4" s="87" t="s">
+      <c r="E4" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="76"/>
-      <c r="I4" s="61" t="s">
+      <c r="H4" s="82"/>
+      <c r="I4" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="87" t="s">
+      <c r="J4" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="K4" s="88" t="s">
+      <c r="K4" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="53">
+      <c r="L4" s="57">
         <v>25070</v>
       </c>
-      <c r="M4" s="70" t="s">
+      <c r="M4" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="N4" s="76"/>
-      <c r="O4" s="57" t="s">
+      <c r="N4" s="82"/>
+      <c r="O4" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="P4" s="53" t="s">
+      <c r="P4" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="Q4" s="55" t="s">
+      <c r="Q4" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="R4" s="66" t="s">
+      <c r="R4" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="S4" s="110" t="s">
+      <c r="S4" s="116" t="s">
         <v>44</v>
       </c>
-      <c r="T4" s="72" t="s">
+      <c r="T4" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="U4" s="51" t="s">
+      <c r="U4" s="55" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="27"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="54"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="77"/>
-      <c r="O5" s="58"/>
-      <c r="P5" s="54"/>
-      <c r="Q5" s="56"/>
-      <c r="R5" s="67"/>
-      <c r="S5" s="111"/>
-      <c r="T5" s="73"/>
-      <c r="U5" s="52"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="95"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="58"/>
+      <c r="Q5" s="60"/>
+      <c r="R5" s="73"/>
+      <c r="S5" s="117"/>
+      <c r="T5" s="79"/>
+      <c r="U5" s="56"/>
     </row>
     <row r="6" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27"/>
-      <c r="B6" s="98">
+      <c r="B6" s="90">
         <v>1</v>
       </c>
-      <c r="C6" s="101">
+      <c r="C6" s="106">
         <v>2</v>
       </c>
-      <c r="D6" s="80">
+      <c r="D6" s="86">
         <v>3</v>
       </c>
-      <c r="E6" s="82" t="s">
+      <c r="E6" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="98" t="s">
+      <c r="F6" s="90" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="80" t="s">
+      <c r="G6" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="90"/>
-      <c r="I6" s="85" t="s">
+      <c r="H6" s="96"/>
+      <c r="I6" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="82" t="s">
+      <c r="J6" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="96" t="s">
+      <c r="K6" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="L6" s="98" t="s">
+      <c r="L6" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="M6" s="80">
+      <c r="M6" s="86">
         <v>25070</v>
       </c>
-      <c r="N6" s="90"/>
-      <c r="O6" s="85" t="s">
+      <c r="N6" s="96"/>
+      <c r="O6" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="P6" s="98" t="s">
+      <c r="P6" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="101" t="s">
+      <c r="Q6" s="106" t="s">
         <v>64</v>
       </c>
-      <c r="R6" s="107" t="s">
+      <c r="R6" s="112" t="s">
         <v>65</v>
       </c>
-      <c r="S6" s="112" t="s">
+      <c r="S6" s="118" t="s">
         <v>51</v>
       </c>
-      <c r="T6" s="99" t="s">
+      <c r="T6" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="U6" s="92" t="s">
+      <c r="U6" s="98" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="27"/>
-      <c r="B7" s="84"/>
-      <c r="C7" s="102"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="83"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="91"/>
-      <c r="I7" s="86"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="97"/>
-      <c r="L7" s="84"/>
-      <c r="M7" s="81"/>
-      <c r="N7" s="91"/>
-      <c r="O7" s="86"/>
-      <c r="P7" s="84"/>
-      <c r="Q7" s="102"/>
-      <c r="R7" s="108"/>
-      <c r="S7" s="113"/>
-      <c r="T7" s="100"/>
-      <c r="U7" s="93"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="97"/>
+      <c r="I7" s="93"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="103"/>
+      <c r="L7" s="91"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="97"/>
+      <c r="O7" s="93"/>
+      <c r="P7" s="91"/>
+      <c r="Q7" s="107"/>
+      <c r="R7" s="113"/>
+      <c r="S7" s="119"/>
+      <c r="T7" s="105"/>
+      <c r="U7" s="99"/>
     </row>
     <row r="8" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="27"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="87"/>
-      <c r="K8" s="88"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="57"/>
-      <c r="N8" s="109"/>
-      <c r="O8" s="94"/>
-      <c r="P8" s="53"/>
-      <c r="Q8" s="55"/>
-      <c r="R8" s="66"/>
-      <c r="S8" s="109"/>
-      <c r="T8" s="94"/>
-      <c r="U8" s="51"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="114"/>
+      <c r="I8" s="100"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="57"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="114"/>
+      <c r="O8" s="100"/>
+      <c r="P8" s="57"/>
+      <c r="Q8" s="59"/>
+      <c r="R8" s="72"/>
+      <c r="S8" s="114"/>
+      <c r="T8" s="100"/>
+      <c r="U8" s="55"/>
     </row>
     <row r="9" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="27"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="95"/>
-      <c r="J9" s="59"/>
-      <c r="K9" s="89"/>
-      <c r="L9" s="54"/>
-      <c r="M9" s="58"/>
-      <c r="N9" s="60"/>
-      <c r="O9" s="95"/>
-      <c r="P9" s="54"/>
-      <c r="Q9" s="56"/>
-      <c r="R9" s="67"/>
-      <c r="S9" s="60"/>
-      <c r="T9" s="95"/>
-      <c r="U9" s="52"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="115"/>
+      <c r="I9" s="101"/>
+      <c r="J9" s="64"/>
+      <c r="K9" s="95"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="62"/>
+      <c r="N9" s="115"/>
+      <c r="O9" s="101"/>
+      <c r="P9" s="58"/>
+      <c r="Q9" s="60"/>
+      <c r="R9" s="73"/>
+      <c r="S9" s="115"/>
+      <c r="T9" s="101"/>
+      <c r="U9" s="56"/>
     </row>
     <row r="10" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27"/>
-      <c r="B10" s="98"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="98"/>
-      <c r="G10" s="80"/>
-      <c r="H10" s="90"/>
-      <c r="I10" s="85"/>
-      <c r="J10" s="82"/>
-      <c r="K10" s="96"/>
-      <c r="L10" s="98"/>
-      <c r="M10" s="80"/>
-      <c r="N10" s="90"/>
-      <c r="O10" s="85"/>
-      <c r="P10" s="98"/>
-      <c r="Q10" s="101"/>
-      <c r="R10" s="107"/>
-      <c r="S10" s="90"/>
-      <c r="T10" s="85"/>
-      <c r="U10" s="92"/>
+      <c r="B10" s="90"/>
+      <c r="C10" s="106"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="90"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="96"/>
+      <c r="I10" s="92"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="90"/>
+      <c r="M10" s="86"/>
+      <c r="N10" s="96"/>
+      <c r="O10" s="92"/>
+      <c r="P10" s="90"/>
+      <c r="Q10" s="106"/>
+      <c r="R10" s="112"/>
+      <c r="S10" s="96"/>
+      <c r="T10" s="92"/>
+      <c r="U10" s="98"/>
     </row>
     <row r="11" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="27"/>
-      <c r="B11" s="84"/>
-      <c r="C11" s="102"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="83"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="91"/>
-      <c r="I11" s="86"/>
-      <c r="J11" s="83"/>
-      <c r="K11" s="97"/>
-      <c r="L11" s="84"/>
-      <c r="M11" s="81"/>
-      <c r="N11" s="91"/>
-      <c r="O11" s="86"/>
-      <c r="P11" s="84"/>
-      <c r="Q11" s="102"/>
-      <c r="R11" s="108"/>
-      <c r="S11" s="91"/>
-      <c r="T11" s="86"/>
-      <c r="U11" s="93"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="107"/>
+      <c r="D11" s="87"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="91"/>
+      <c r="G11" s="87"/>
+      <c r="H11" s="97"/>
+      <c r="I11" s="93"/>
+      <c r="J11" s="89"/>
+      <c r="K11" s="103"/>
+      <c r="L11" s="91"/>
+      <c r="M11" s="87"/>
+      <c r="N11" s="97"/>
+      <c r="O11" s="93"/>
+      <c r="P11" s="91"/>
+      <c r="Q11" s="107"/>
+      <c r="R11" s="113"/>
+      <c r="S11" s="97"/>
+      <c r="T11" s="93"/>
+      <c r="U11" s="99"/>
     </row>
     <row r="12" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="87"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="109"/>
-      <c r="I12" s="94"/>
-      <c r="J12" s="87"/>
-      <c r="K12" s="88"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="57"/>
-      <c r="N12" s="109"/>
-      <c r="O12" s="94"/>
-      <c r="P12" s="53"/>
-      <c r="Q12" s="55"/>
-      <c r="R12" s="66"/>
-      <c r="S12" s="109"/>
-      <c r="T12" s="94"/>
-      <c r="U12" s="51"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="114"/>
+      <c r="I12" s="100"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="94"/>
+      <c r="L12" s="57"/>
+      <c r="M12" s="61"/>
+      <c r="N12" s="114"/>
+      <c r="O12" s="100"/>
+      <c r="P12" s="57"/>
+      <c r="Q12" s="59"/>
+      <c r="R12" s="72"/>
+      <c r="S12" s="114"/>
+      <c r="T12" s="100"/>
+      <c r="U12" s="55"/>
     </row>
     <row r="13" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="27"/>
-      <c r="B13" s="54"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="95"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="89"/>
-      <c r="L13" s="54"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="95"/>
-      <c r="P13" s="54"/>
-      <c r="Q13" s="56"/>
-      <c r="R13" s="67"/>
-      <c r="S13" s="60"/>
-      <c r="T13" s="95"/>
-      <c r="U13" s="52"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="115"/>
+      <c r="I13" s="101"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="95"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="115"/>
+      <c r="O13" s="101"/>
+      <c r="P13" s="58"/>
+      <c r="Q13" s="60"/>
+      <c r="R13" s="73"/>
+      <c r="S13" s="115"/>
+      <c r="T13" s="101"/>
+      <c r="U13" s="56"/>
     </row>
     <row r="14" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="27"/>
-      <c r="B14" s="98"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="82"/>
-      <c r="F14" s="98"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="90"/>
-      <c r="I14" s="85"/>
-      <c r="J14" s="82"/>
-      <c r="K14" s="96"/>
-      <c r="L14" s="98"/>
-      <c r="M14" s="80"/>
-      <c r="N14" s="90"/>
-      <c r="O14" s="85"/>
-      <c r="P14" s="98"/>
-      <c r="Q14" s="101"/>
-      <c r="R14" s="107"/>
-      <c r="S14" s="90"/>
-      <c r="T14" s="85"/>
-      <c r="U14" s="92"/>
+      <c r="B14" s="90"/>
+      <c r="C14" s="106"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="96"/>
+      <c r="I14" s="92"/>
+      <c r="J14" s="88"/>
+      <c r="K14" s="102"/>
+      <c r="L14" s="90"/>
+      <c r="M14" s="86"/>
+      <c r="N14" s="96"/>
+      <c r="O14" s="92"/>
+      <c r="P14" s="90"/>
+      <c r="Q14" s="106"/>
+      <c r="R14" s="112"/>
+      <c r="S14" s="96"/>
+      <c r="T14" s="92"/>
+      <c r="U14" s="98"/>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="27"/>
-      <c r="B15" s="84"/>
-      <c r="C15" s="102"/>
-      <c r="D15" s="81"/>
-      <c r="E15" s="83"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="81"/>
-      <c r="H15" s="91"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="83"/>
-      <c r="K15" s="97"/>
-      <c r="L15" s="84"/>
-      <c r="M15" s="81"/>
-      <c r="N15" s="91"/>
-      <c r="O15" s="86"/>
-      <c r="P15" s="84"/>
-      <c r="Q15" s="102"/>
-      <c r="R15" s="108"/>
-      <c r="S15" s="91"/>
-      <c r="T15" s="86"/>
-      <c r="U15" s="93"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="107"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="89"/>
+      <c r="F15" s="91"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="97"/>
+      <c r="I15" s="93"/>
+      <c r="J15" s="89"/>
+      <c r="K15" s="103"/>
+      <c r="L15" s="91"/>
+      <c r="M15" s="87"/>
+      <c r="N15" s="97"/>
+      <c r="O15" s="93"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="107"/>
+      <c r="R15" s="113"/>
+      <c r="S15" s="97"/>
+      <c r="T15" s="93"/>
+      <c r="U15" s="99"/>
     </row>
     <row r="16" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="27"/>
-      <c r="B16" s="53"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="87"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="109"/>
-      <c r="I16" s="94"/>
-      <c r="J16" s="87"/>
-      <c r="K16" s="88"/>
-      <c r="L16" s="53"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="109"/>
-      <c r="O16" s="94"/>
-      <c r="P16" s="53"/>
-      <c r="Q16" s="55"/>
-      <c r="R16" s="66"/>
-      <c r="S16" s="109"/>
-      <c r="T16" s="94"/>
-      <c r="U16" s="51"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="114"/>
+      <c r="I16" s="100"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="94"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="61"/>
+      <c r="N16" s="114"/>
+      <c r="O16" s="100"/>
+      <c r="P16" s="57"/>
+      <c r="Q16" s="59"/>
+      <c r="R16" s="72"/>
+      <c r="S16" s="114"/>
+      <c r="T16" s="100"/>
+      <c r="U16" s="55"/>
     </row>
     <row r="17" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="27"/>
-      <c r="B17" s="54"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="103"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="89"/>
-      <c r="L17" s="54"/>
-      <c r="M17" s="58"/>
-      <c r="N17" s="60"/>
-      <c r="O17" s="103"/>
-      <c r="P17" s="54"/>
-      <c r="Q17" s="56"/>
-      <c r="R17" s="67"/>
-      <c r="S17" s="60"/>
-      <c r="T17" s="103"/>
-      <c r="U17" s="104"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="115"/>
+      <c r="I17" s="108"/>
+      <c r="J17" s="64"/>
+      <c r="K17" s="95"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="62"/>
+      <c r="N17" s="115"/>
+      <c r="O17" s="108"/>
+      <c r="P17" s="58"/>
+      <c r="Q17" s="60"/>
+      <c r="R17" s="73"/>
+      <c r="S17" s="115"/>
+      <c r="T17" s="108"/>
+      <c r="U17" s="109"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="27"/>
@@ -2653,7 +2713,7 @@
   <dimension ref="B1:T21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:L5"/>
+      <selection activeCell="Q4" sqref="Q4:Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2673,41 +2733,41 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:20" ht="19.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="40" t="s">
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="41"/>
-      <c r="M2" s="42" t="s">
+      <c r="L2" s="69"/>
+      <c r="M2" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="43" t="s">
+      <c r="N2" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="O2" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="43" t="s">
+      <c r="P2" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="44" t="s">
+      <c r="Q2" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="74" t="s">
+      <c r="R2" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="S2" s="75"/>
-      <c r="T2" s="141" t="s">
+      <c r="S2" s="81"/>
+      <c r="T2" s="152" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2745,359 +2805,360 @@
       <c r="L3" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="42"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="44"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="38"/>
       <c r="R3" s="24" t="s">
         <v>36</v>
       </c>
       <c r="S3" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="T3" s="141"/>
+      <c r="T3" s="152"/>
     </row>
     <row r="4" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="47">
+      <c r="B4" s="44">
         <f>IF(K4&gt;0, C4/K4,"RF")</f>
         <v>-9.9261059795819158</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="36">
         <f>(D4/P4)-1</f>
         <v>-1</v>
       </c>
-      <c r="D4" s="48">
+      <c r="D4" s="45">
         <v>0</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="44">
         <f>IF(K4&gt;0, F4/K4,"RF")</f>
         <v>4.124939231891104</v>
       </c>
-      <c r="F4" s="35">
+      <c r="F4" s="36">
         <f>(G4/P4)-1</f>
         <v>0.41556469781565286</v>
       </c>
-      <c r="G4" s="48">
+      <c r="G4" s="45">
         <v>28903</v>
       </c>
-      <c r="H4" s="47">
+      <c r="H4" s="44">
         <f>IF(K4&gt;0, I4/K4,"RF")</f>
         <v>3.068546426835197</v>
       </c>
-      <c r="I4" s="35">
+      <c r="I4" s="36">
         <f>(J4/P4)-1</f>
         <v>0.30913899500440789</v>
       </c>
-      <c r="J4" s="48">
+      <c r="J4" s="45">
         <v>26730</v>
       </c>
-      <c r="K4" s="49">
+      <c r="K4" s="169">
         <f>IF(1-(L4/P4)&gt;0, 1-(L4/P4), 0)</f>
         <v>0.10074444117935155</v>
       </c>
-      <c r="L4" s="50">
+      <c r="L4" s="46">
         <v>18361</v>
       </c>
-      <c r="M4" s="34">
+      <c r="M4" s="35">
         <f>P4*Q4</f>
         <v>69543708</v>
       </c>
-      <c r="N4" s="35">
+      <c r="N4" s="36">
         <f>IF( (P4-L4)*Q4/O4&gt;0, (P4-L4)*Q4/O4, "Risk free")</f>
-        <v>1.1120860317460318E-2</v>
-      </c>
-      <c r="O4" s="36">
-        <v>630000000</v>
-      </c>
-      <c r="P4" s="36">
+        <v>4.6372783012632226E-3</v>
+      </c>
+      <c r="O4" s="37">
+        <f>'[1]مدیریت سرمایه'!$B$5</f>
+        <v>1510830609</v>
+      </c>
+      <c r="P4" s="150">
         <v>20418</v>
       </c>
-      <c r="Q4" s="138">
+      <c r="Q4" s="147">
         <v>3406</v>
       </c>
-      <c r="R4" s="110" t="s">
+      <c r="R4" s="116" t="s">
         <v>44</v>
       </c>
-      <c r="S4" s="61" t="s">
+      <c r="S4" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="T4" s="46" t="s">
+      <c r="T4" s="34" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="47"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="138"/>
-      <c r="R5" s="111"/>
-      <c r="S5" s="62"/>
-      <c r="T5" s="46"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="169"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="150"/>
+      <c r="Q5" s="147"/>
+      <c r="R5" s="117"/>
+      <c r="S5" s="66"/>
+      <c r="T5" s="34"/>
     </row>
     <row r="6" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="47"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="36"/>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="138"/>
-      <c r="R6" s="139"/>
-      <c r="S6" s="61"/>
-      <c r="T6" s="46"/>
+      <c r="B6" s="151"/>
+      <c r="C6" s="146"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="151"/>
+      <c r="F6" s="146"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="151"/>
+      <c r="I6" s="146"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="144"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="145"/>
+      <c r="N6" s="146"/>
+      <c r="O6" s="150"/>
+      <c r="P6" s="150"/>
+      <c r="Q6" s="147"/>
+      <c r="R6" s="148"/>
+      <c r="S6" s="65"/>
+      <c r="T6" s="34"/>
     </row>
     <row r="7" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="47"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="36"/>
-      <c r="Q7" s="138"/>
-      <c r="R7" s="140"/>
-      <c r="S7" s="62"/>
-      <c r="T7" s="46"/>
+      <c r="B7" s="151"/>
+      <c r="C7" s="146"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="151"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="151"/>
+      <c r="I7" s="146"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="144"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="145"/>
+      <c r="N7" s="146"/>
+      <c r="O7" s="150"/>
+      <c r="P7" s="150"/>
+      <c r="Q7" s="147"/>
+      <c r="R7" s="149"/>
+      <c r="S7" s="66"/>
+      <c r="T7" s="34"/>
     </row>
     <row r="8" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="124"/>
-      <c r="C8" s="116"/>
-      <c r="D8" s="118"/>
-      <c r="E8" s="124"/>
-      <c r="F8" s="116"/>
-      <c r="G8" s="118"/>
-      <c r="H8" s="124"/>
-      <c r="I8" s="116"/>
-      <c r="J8" s="118"/>
-      <c r="K8" s="124"/>
-      <c r="L8" s="118"/>
-      <c r="M8" s="124"/>
-      <c r="N8" s="116"/>
-      <c r="O8" s="116"/>
-      <c r="P8" s="116"/>
-      <c r="Q8" s="118"/>
-      <c r="R8" s="120"/>
-      <c r="S8" s="94"/>
-      <c r="T8" s="114"/>
+      <c r="B8" s="130"/>
+      <c r="C8" s="122"/>
+      <c r="D8" s="124"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="122"/>
+      <c r="G8" s="124"/>
+      <c r="H8" s="130"/>
+      <c r="I8" s="122"/>
+      <c r="J8" s="124"/>
+      <c r="K8" s="130"/>
+      <c r="L8" s="124"/>
+      <c r="M8" s="130"/>
+      <c r="N8" s="122"/>
+      <c r="O8" s="122"/>
+      <c r="P8" s="122"/>
+      <c r="Q8" s="124"/>
+      <c r="R8" s="126"/>
+      <c r="S8" s="100"/>
+      <c r="T8" s="120"/>
     </row>
     <row r="9" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="125"/>
-      <c r="C9" s="117"/>
-      <c r="D9" s="119"/>
-      <c r="E9" s="125"/>
-      <c r="F9" s="117"/>
-      <c r="G9" s="119"/>
-      <c r="H9" s="125"/>
-      <c r="I9" s="117"/>
-      <c r="J9" s="119"/>
-      <c r="K9" s="125"/>
-      <c r="L9" s="119"/>
-      <c r="M9" s="125"/>
-      <c r="N9" s="117"/>
-      <c r="O9" s="117"/>
-      <c r="P9" s="117"/>
-      <c r="Q9" s="119"/>
-      <c r="R9" s="121"/>
-      <c r="S9" s="95"/>
-      <c r="T9" s="115"/>
+      <c r="B9" s="131"/>
+      <c r="C9" s="123"/>
+      <c r="D9" s="125"/>
+      <c r="E9" s="131"/>
+      <c r="F9" s="123"/>
+      <c r="G9" s="125"/>
+      <c r="H9" s="131"/>
+      <c r="I9" s="123"/>
+      <c r="J9" s="125"/>
+      <c r="K9" s="131"/>
+      <c r="L9" s="125"/>
+      <c r="M9" s="131"/>
+      <c r="N9" s="123"/>
+      <c r="O9" s="123"/>
+      <c r="P9" s="123"/>
+      <c r="Q9" s="125"/>
+      <c r="R9" s="127"/>
+      <c r="S9" s="101"/>
+      <c r="T9" s="121"/>
     </row>
     <row r="10" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="130"/>
-      <c r="C10" s="132"/>
-      <c r="D10" s="134"/>
-      <c r="E10" s="130"/>
-      <c r="F10" s="132"/>
-      <c r="G10" s="134"/>
-      <c r="H10" s="130"/>
-      <c r="I10" s="132"/>
-      <c r="J10" s="134"/>
-      <c r="K10" s="130"/>
-      <c r="L10" s="134"/>
-      <c r="M10" s="130"/>
-      <c r="N10" s="132"/>
-      <c r="O10" s="132"/>
-      <c r="P10" s="132"/>
-      <c r="Q10" s="134"/>
-      <c r="R10" s="136"/>
-      <c r="S10" s="126"/>
-      <c r="T10" s="128"/>
+      <c r="B10" s="132"/>
+      <c r="C10" s="134"/>
+      <c r="D10" s="136"/>
+      <c r="E10" s="132"/>
+      <c r="F10" s="134"/>
+      <c r="G10" s="136"/>
+      <c r="H10" s="132"/>
+      <c r="I10" s="134"/>
+      <c r="J10" s="136"/>
+      <c r="K10" s="132"/>
+      <c r="L10" s="136"/>
+      <c r="M10" s="132"/>
+      <c r="N10" s="134"/>
+      <c r="O10" s="134"/>
+      <c r="P10" s="134"/>
+      <c r="Q10" s="136"/>
+      <c r="R10" s="142"/>
+      <c r="S10" s="138"/>
+      <c r="T10" s="140"/>
     </row>
     <row r="11" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="131"/>
-      <c r="C11" s="133"/>
-      <c r="D11" s="135"/>
-      <c r="E11" s="131"/>
-      <c r="F11" s="133"/>
-      <c r="G11" s="135"/>
-      <c r="H11" s="131"/>
-      <c r="I11" s="133"/>
-      <c r="J11" s="135"/>
-      <c r="K11" s="131"/>
-      <c r="L11" s="135"/>
-      <c r="M11" s="131"/>
-      <c r="N11" s="133"/>
-      <c r="O11" s="133"/>
-      <c r="P11" s="133"/>
-      <c r="Q11" s="135"/>
-      <c r="R11" s="137"/>
-      <c r="S11" s="127"/>
-      <c r="T11" s="129"/>
+      <c r="B11" s="133"/>
+      <c r="C11" s="135"/>
+      <c r="D11" s="137"/>
+      <c r="E11" s="133"/>
+      <c r="F11" s="135"/>
+      <c r="G11" s="137"/>
+      <c r="H11" s="133"/>
+      <c r="I11" s="135"/>
+      <c r="J11" s="137"/>
+      <c r="K11" s="133"/>
+      <c r="L11" s="137"/>
+      <c r="M11" s="133"/>
+      <c r="N11" s="135"/>
+      <c r="O11" s="135"/>
+      <c r="P11" s="135"/>
+      <c r="Q11" s="137"/>
+      <c r="R11" s="143"/>
+      <c r="S11" s="139"/>
+      <c r="T11" s="141"/>
     </row>
     <row r="12" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="124"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="118"/>
-      <c r="E12" s="124"/>
-      <c r="F12" s="116"/>
-      <c r="G12" s="118"/>
-      <c r="H12" s="124"/>
-      <c r="I12" s="116"/>
-      <c r="J12" s="118"/>
-      <c r="K12" s="124"/>
-      <c r="L12" s="118"/>
-      <c r="M12" s="124"/>
-      <c r="N12" s="116"/>
-      <c r="O12" s="116"/>
-      <c r="P12" s="116"/>
-      <c r="Q12" s="118"/>
-      <c r="R12" s="120"/>
-      <c r="S12" s="122"/>
-      <c r="T12" s="114"/>
+      <c r="B12" s="130"/>
+      <c r="C12" s="122"/>
+      <c r="D12" s="124"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="122"/>
+      <c r="G12" s="124"/>
+      <c r="H12" s="130"/>
+      <c r="I12" s="122"/>
+      <c r="J12" s="124"/>
+      <c r="K12" s="130"/>
+      <c r="L12" s="124"/>
+      <c r="M12" s="130"/>
+      <c r="N12" s="122"/>
+      <c r="O12" s="122"/>
+      <c r="P12" s="122"/>
+      <c r="Q12" s="124"/>
+      <c r="R12" s="126"/>
+      <c r="S12" s="128"/>
+      <c r="T12" s="120"/>
     </row>
     <row r="13" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="125"/>
-      <c r="C13" s="117"/>
-      <c r="D13" s="119"/>
-      <c r="E13" s="125"/>
-      <c r="F13" s="117"/>
-      <c r="G13" s="119"/>
-      <c r="H13" s="125"/>
-      <c r="I13" s="117"/>
-      <c r="J13" s="119"/>
-      <c r="K13" s="125"/>
-      <c r="L13" s="119"/>
-      <c r="M13" s="125"/>
-      <c r="N13" s="117"/>
-      <c r="O13" s="117"/>
-      <c r="P13" s="117"/>
-      <c r="Q13" s="119"/>
-      <c r="R13" s="121"/>
-      <c r="S13" s="123"/>
-      <c r="T13" s="115"/>
+      <c r="B13" s="131"/>
+      <c r="C13" s="123"/>
+      <c r="D13" s="125"/>
+      <c r="E13" s="131"/>
+      <c r="F13" s="123"/>
+      <c r="G13" s="125"/>
+      <c r="H13" s="131"/>
+      <c r="I13" s="123"/>
+      <c r="J13" s="125"/>
+      <c r="K13" s="131"/>
+      <c r="L13" s="125"/>
+      <c r="M13" s="131"/>
+      <c r="N13" s="123"/>
+      <c r="O13" s="123"/>
+      <c r="P13" s="123"/>
+      <c r="Q13" s="125"/>
+      <c r="R13" s="127"/>
+      <c r="S13" s="129"/>
+      <c r="T13" s="121"/>
     </row>
     <row r="14" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="130"/>
-      <c r="C14" s="132"/>
-      <c r="D14" s="134"/>
-      <c r="E14" s="130"/>
-      <c r="F14" s="132"/>
-      <c r="G14" s="134"/>
-      <c r="H14" s="130"/>
-      <c r="I14" s="132"/>
-      <c r="J14" s="134"/>
-      <c r="K14" s="130"/>
-      <c r="L14" s="134"/>
-      <c r="M14" s="130"/>
-      <c r="N14" s="132"/>
-      <c r="O14" s="132"/>
-      <c r="P14" s="132"/>
-      <c r="Q14" s="134"/>
-      <c r="R14" s="136"/>
-      <c r="S14" s="126"/>
-      <c r="T14" s="128"/>
+      <c r="B14" s="132"/>
+      <c r="C14" s="134"/>
+      <c r="D14" s="136"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="134"/>
+      <c r="G14" s="136"/>
+      <c r="H14" s="132"/>
+      <c r="I14" s="134"/>
+      <c r="J14" s="136"/>
+      <c r="K14" s="132"/>
+      <c r="L14" s="136"/>
+      <c r="M14" s="132"/>
+      <c r="N14" s="134"/>
+      <c r="O14" s="134"/>
+      <c r="P14" s="134"/>
+      <c r="Q14" s="136"/>
+      <c r="R14" s="142"/>
+      <c r="S14" s="138"/>
+      <c r="T14" s="140"/>
     </row>
     <row r="15" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="131"/>
-      <c r="C15" s="133"/>
-      <c r="D15" s="135"/>
-      <c r="E15" s="131"/>
-      <c r="F15" s="133"/>
-      <c r="G15" s="135"/>
-      <c r="H15" s="131"/>
-      <c r="I15" s="133"/>
-      <c r="J15" s="135"/>
-      <c r="K15" s="131"/>
-      <c r="L15" s="135"/>
-      <c r="M15" s="131"/>
-      <c r="N15" s="133"/>
-      <c r="O15" s="133"/>
-      <c r="P15" s="133"/>
-      <c r="Q15" s="135"/>
-      <c r="R15" s="137"/>
-      <c r="S15" s="127"/>
-      <c r="T15" s="129"/>
+      <c r="B15" s="133"/>
+      <c r="C15" s="135"/>
+      <c r="D15" s="137"/>
+      <c r="E15" s="133"/>
+      <c r="F15" s="135"/>
+      <c r="G15" s="137"/>
+      <c r="H15" s="133"/>
+      <c r="I15" s="135"/>
+      <c r="J15" s="137"/>
+      <c r="K15" s="133"/>
+      <c r="L15" s="137"/>
+      <c r="M15" s="133"/>
+      <c r="N15" s="135"/>
+      <c r="O15" s="135"/>
+      <c r="P15" s="135"/>
+      <c r="Q15" s="137"/>
+      <c r="R15" s="143"/>
+      <c r="S15" s="139"/>
+      <c r="T15" s="141"/>
     </row>
     <row r="16" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="124"/>
-      <c r="C16" s="116"/>
-      <c r="D16" s="118"/>
-      <c r="E16" s="124"/>
-      <c r="F16" s="116"/>
-      <c r="G16" s="118"/>
-      <c r="H16" s="124"/>
-      <c r="I16" s="116"/>
-      <c r="J16" s="118"/>
-      <c r="K16" s="124"/>
-      <c r="L16" s="118"/>
-      <c r="M16" s="124"/>
-      <c r="N16" s="116"/>
-      <c r="O16" s="116"/>
-      <c r="P16" s="116"/>
-      <c r="Q16" s="118"/>
-      <c r="R16" s="120"/>
-      <c r="S16" s="122"/>
-      <c r="T16" s="114"/>
+      <c r="B16" s="130"/>
+      <c r="C16" s="122"/>
+      <c r="D16" s="124"/>
+      <c r="E16" s="130"/>
+      <c r="F16" s="122"/>
+      <c r="G16" s="124"/>
+      <c r="H16" s="130"/>
+      <c r="I16" s="122"/>
+      <c r="J16" s="124"/>
+      <c r="K16" s="130"/>
+      <c r="L16" s="124"/>
+      <c r="M16" s="130"/>
+      <c r="N16" s="122"/>
+      <c r="O16" s="122"/>
+      <c r="P16" s="122"/>
+      <c r="Q16" s="124"/>
+      <c r="R16" s="126"/>
+      <c r="S16" s="128"/>
+      <c r="T16" s="120"/>
     </row>
     <row r="17" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="125"/>
-      <c r="C17" s="117"/>
-      <c r="D17" s="119"/>
-      <c r="E17" s="125"/>
-      <c r="F17" s="117"/>
-      <c r="G17" s="119"/>
-      <c r="H17" s="125"/>
-      <c r="I17" s="117"/>
-      <c r="J17" s="119"/>
-      <c r="K17" s="125"/>
-      <c r="L17" s="119"/>
-      <c r="M17" s="125"/>
-      <c r="N17" s="117"/>
-      <c r="O17" s="117"/>
-      <c r="P17" s="117"/>
-      <c r="Q17" s="119"/>
-      <c r="R17" s="121"/>
-      <c r="S17" s="123"/>
-      <c r="T17" s="115"/>
+      <c r="B17" s="131"/>
+      <c r="C17" s="123"/>
+      <c r="D17" s="125"/>
+      <c r="E17" s="131"/>
+      <c r="F17" s="123"/>
+      <c r="G17" s="125"/>
+      <c r="H17" s="131"/>
+      <c r="I17" s="123"/>
+      <c r="J17" s="125"/>
+      <c r="K17" s="131"/>
+      <c r="L17" s="125"/>
+      <c r="M17" s="131"/>
+      <c r="N17" s="123"/>
+      <c r="O17" s="123"/>
+      <c r="P17" s="123"/>
+      <c r="Q17" s="125"/>
+      <c r="R17" s="127"/>
+      <c r="S17" s="129"/>
+      <c r="T17" s="121"/>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S20" s="31"/>
@@ -3126,6 +3187,13 @@
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="T4:T5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
@@ -3135,13 +3203,6 @@
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="L4:L5"/>
     <mergeCell ref="M4:M5"/>
@@ -3163,6 +3224,9 @@
     <mergeCell ref="P6:P7"/>
     <mergeCell ref="S8:S9"/>
     <mergeCell ref="T8:T9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>
@@ -3172,9 +3236,10 @@
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="N10:N11"/>
     <mergeCell ref="R8:R9"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="H8:H9"/>
@@ -3199,10 +3264,6 @@
     <mergeCell ref="S10:S11"/>
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="N10:N11"/>
     <mergeCell ref="Q12:Q13"/>
     <mergeCell ref="R12:R13"/>
     <mergeCell ref="S12:S13"/>
@@ -3220,6 +3281,10 @@
     <mergeCell ref="P12:P13"/>
     <mergeCell ref="S14:S15"/>
     <mergeCell ref="T14:T15"/>
+    <mergeCell ref="O14:O15"/>
+    <mergeCell ref="P14:P15"/>
+    <mergeCell ref="Q14:Q15"/>
+    <mergeCell ref="R14:R15"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="D16:D17"/>
@@ -3229,10 +3294,6 @@
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="M14:M15"/>
     <mergeCell ref="N14:N15"/>
-    <mergeCell ref="O14:O15"/>
-    <mergeCell ref="P14:P15"/>
-    <mergeCell ref="Q14:Q15"/>
-    <mergeCell ref="R14:R15"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="I14:I15"/>
@@ -3263,9 +3324,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4:H5"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3283,155 +3344,155 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:10" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="141" t="s">
+      <c r="C2" s="152" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="141" t="s">
+      <c r="E2" s="152" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="149" t="s">
+      <c r="F2" s="160" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="141" t="s">
+      <c r="G2" s="152" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="156" t="s">
+      <c r="H2" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="157"/>
-      <c r="J2" s="141" t="s">
+      <c r="I2" s="49"/>
+      <c r="J2" s="152" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="32"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="141"/>
-      <c r="F3" s="150"/>
-      <c r="G3" s="42"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="161"/>
+      <c r="G3" s="40"/>
       <c r="H3" s="29" t="s">
         <v>39</v>
       </c>
       <c r="I3" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="141"/>
+      <c r="J3" s="152"/>
     </row>
     <row r="4" spans="2:10" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="146">
+      <c r="B4" s="167">
         <f>D4-(F4*G4)</f>
         <v>4378033</v>
       </c>
-      <c r="C4" s="147">
+      <c r="C4" s="168">
         <f>E4/F4-1</f>
         <v>0.28176119110588704</v>
       </c>
-      <c r="D4" s="146">
+      <c r="D4" s="167">
         <f>E4*G4</f>
         <v>19916131</v>
       </c>
-      <c r="E4" s="146">
+      <c r="E4" s="157">
         <v>26171</v>
       </c>
-      <c r="F4" s="151">
+      <c r="F4" s="162">
         <v>20418</v>
       </c>
-      <c r="G4" s="148">
+      <c r="G4" s="159">
         <v>761</v>
       </c>
-      <c r="H4" s="142" t="s">
+      <c r="H4" s="153" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="155" t="s">
+      <c r="I4" s="166" t="s">
         <v>66</v>
       </c>
-      <c r="J4" s="148" t="s">
+      <c r="J4" s="159" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="146"/>
-      <c r="C5" s="147"/>
-      <c r="D5" s="146"/>
-      <c r="E5" s="146"/>
-      <c r="F5" s="152"/>
-      <c r="G5" s="148"/>
-      <c r="H5" s="143"/>
-      <c r="I5" s="155"/>
-      <c r="J5" s="148"/>
+      <c r="B5" s="167"/>
+      <c r="C5" s="168"/>
+      <c r="D5" s="167"/>
+      <c r="E5" s="157"/>
+      <c r="F5" s="163"/>
+      <c r="G5" s="159"/>
+      <c r="H5" s="154"/>
+      <c r="I5" s="166"/>
+      <c r="J5" s="159"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="146"/>
-      <c r="C6" s="147"/>
-      <c r="D6" s="146"/>
-      <c r="E6" s="146"/>
-      <c r="F6" s="151"/>
-      <c r="G6" s="148"/>
-      <c r="H6" s="142"/>
-      <c r="I6" s="155"/>
-      <c r="J6" s="148"/>
+      <c r="B6" s="157"/>
+      <c r="C6" s="158"/>
+      <c r="D6" s="157"/>
+      <c r="E6" s="157"/>
+      <c r="F6" s="162"/>
+      <c r="G6" s="159"/>
+      <c r="H6" s="153"/>
+      <c r="I6" s="166"/>
+      <c r="J6" s="159"/>
     </row>
     <row r="7" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="146"/>
-      <c r="C7" s="147"/>
-      <c r="D7" s="146"/>
-      <c r="E7" s="146"/>
-      <c r="F7" s="152"/>
-      <c r="G7" s="148"/>
-      <c r="H7" s="143"/>
-      <c r="I7" s="155"/>
-      <c r="J7" s="148"/>
+      <c r="B7" s="157"/>
+      <c r="C7" s="158"/>
+      <c r="D7" s="157"/>
+      <c r="E7" s="157"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="159"/>
+      <c r="H7" s="154"/>
+      <c r="I7" s="166"/>
+      <c r="J7" s="159"/>
     </row>
     <row r="8" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="148"/>
-      <c r="C8" s="148"/>
-      <c r="D8" s="148"/>
-      <c r="E8" s="148"/>
-      <c r="F8" s="153"/>
-      <c r="G8" s="148"/>
-      <c r="H8" s="144"/>
-      <c r="I8" s="155"/>
-      <c r="J8" s="148"/>
+      <c r="B8" s="159"/>
+      <c r="C8" s="159"/>
+      <c r="D8" s="159"/>
+      <c r="E8" s="159"/>
+      <c r="F8" s="164"/>
+      <c r="G8" s="159"/>
+      <c r="H8" s="155"/>
+      <c r="I8" s="166"/>
+      <c r="J8" s="159"/>
     </row>
     <row r="9" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="148"/>
-      <c r="C9" s="148"/>
-      <c r="D9" s="148"/>
-      <c r="E9" s="148"/>
-      <c r="F9" s="154"/>
-      <c r="G9" s="148"/>
-      <c r="H9" s="145"/>
-      <c r="I9" s="155"/>
-      <c r="J9" s="148"/>
+      <c r="B9" s="159"/>
+      <c r="C9" s="159"/>
+      <c r="D9" s="159"/>
+      <c r="E9" s="159"/>
+      <c r="F9" s="165"/>
+      <c r="G9" s="159"/>
+      <c r="H9" s="156"/>
+      <c r="I9" s="166"/>
+      <c r="J9" s="159"/>
     </row>
     <row r="10" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="148"/>
-      <c r="C10" s="148"/>
-      <c r="D10" s="148"/>
-      <c r="E10" s="148"/>
-      <c r="F10" s="153"/>
-      <c r="G10" s="148"/>
-      <c r="H10" s="144"/>
-      <c r="I10" s="155"/>
-      <c r="J10" s="148"/>
+      <c r="B10" s="159"/>
+      <c r="C10" s="159"/>
+      <c r="D10" s="159"/>
+      <c r="E10" s="159"/>
+      <c r="F10" s="164"/>
+      <c r="G10" s="159"/>
+      <c r="H10" s="155"/>
+      <c r="I10" s="166"/>
+      <c r="J10" s="159"/>
     </row>
     <row r="11" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="148"/>
-      <c r="C11" s="148"/>
-      <c r="D11" s="148"/>
-      <c r="E11" s="148"/>
-      <c r="F11" s="154"/>
-      <c r="G11" s="148"/>
-      <c r="H11" s="145"/>
-      <c r="I11" s="155"/>
-      <c r="J11" s="148"/>
+      <c r="B11" s="159"/>
+      <c r="C11" s="159"/>
+      <c r="D11" s="159"/>
+      <c r="E11" s="159"/>
+      <c r="F11" s="165"/>
+      <c r="G11" s="159"/>
+      <c r="H11" s="156"/>
+      <c r="I11" s="166"/>
+      <c r="J11" s="159"/>
     </row>
   </sheetData>
   <mergeCells count="44">

</xml_diff>